<commit_message>
added district personal income into the database along with scripts
</commit_message>
<xml_diff>
--- a/data/FinancialData/FinancialDataElements/PersonalIncome/Personal Income 2020.xlsx
+++ b/data/FinancialData/FinancialDataElements/PersonalIncome/Personal Income 2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pagov-my.sharepoint.com/personal/bheimbach_pa_gov/Documents/Desktop/Web Dump/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlynch/cs320/dbms_proj/data/FinancialData/FinancialDataElements/PersonalIncome/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FBB8E98F-DD52-4760-8B8B-C7D89FB7B7D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F6E1F9-B798-3A46-8CFB-23889E72916F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4830" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4840" yWindow="4220" windowWidth="21600" windowHeight="11380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Personal Income 2020" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="datamay26" type="6" refreshedVersion="1" background="1" saveData="1">
-    <textPr codePage="28603" sourceFile="H:\shbrady C drive\ACT 80\datamay26.txt" delimited="0">
+    <textPr sourceFile="H:\shbrady C drive\ACT 80\datamay26.txt" delimited="0">
       <textFields count="10">
         <textField/>
         <textField position="5"/>
@@ -1791,16 +1791,15 @@
     <t xml:space="preserve">Tamaqua Area SD </t>
   </si>
   <si>
+    <t>River Valley SD</t>
+  </si>
+  <si>
+    <t>Knoch SD</t>
+  </si>
+  <si>
     <t>Adjusted
 Personal
-Income
-June 2022</t>
-  </si>
-  <si>
-    <t>River Valley SD</t>
-  </si>
-  <si>
-    <t>Knoch SD</t>
+Income</t>
   </si>
 </sst>
 </file>
@@ -1922,9 +1921,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1962,9 +1961,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1997,26 +1996,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2049,26 +2031,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2248,25 +2213,25 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="12.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="10"/>
+    <col min="4" max="4" width="7.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="12.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="13.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.1640625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="5" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2304,10 +2269,10 @@
         <v>454</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <v>112011103</v>
       </c>
@@ -2348,7 +2313,7 @@
         <v>383282319</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A3" s="6">
         <v>112011603</v>
       </c>
@@ -2389,7 +2354,7 @@
         <v>784270948</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A4" s="6">
         <v>112013054</v>
       </c>
@@ -2430,7 +2395,7 @@
         <v>240523853</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A5" s="6">
         <v>112013753</v>
       </c>
@@ -2471,7 +2436,7 @@
         <v>730039655</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A6" s="6">
         <v>112015203</v>
       </c>
@@ -2512,7 +2477,7 @@
         <v>404793973</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A7" s="6">
         <v>112018523</v>
       </c>
@@ -2553,7 +2518,7 @@
         <v>301576086</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A8" s="6">
         <v>103020603</v>
       </c>
@@ -2594,7 +2559,7 @@
         <v>302912508</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A9" s="6">
         <v>103020753</v>
       </c>
@@ -2635,7 +2600,7 @@
         <v>622152213</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A10" s="6">
         <v>103021102</v>
       </c>
@@ -2676,7 +2641,7 @@
         <v>1033734982</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A11" s="6">
         <v>103021252</v>
       </c>
@@ -2717,7 +2682,7 @@
         <v>1146901271</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A12" s="6">
         <v>103021453</v>
       </c>
@@ -2758,7 +2723,7 @@
         <v>245025661</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A13" s="6">
         <v>103021603</v>
       </c>
@@ -2799,7 +2764,7 @@
         <v>393889926</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A14" s="6">
         <v>103021752</v>
       </c>
@@ -2840,7 +2805,7 @@
         <v>1183049981</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A15" s="6">
         <v>103021903</v>
       </c>
@@ -2881,7 +2846,7 @@
         <v>84065672</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A16" s="6">
         <v>103022103</v>
       </c>
@@ -2922,7 +2887,7 @@
         <v>146533610</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A17" s="6">
         <v>103022253</v>
       </c>
@@ -2963,7 +2928,7 @@
         <v>410257988</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A18" s="6">
         <v>103022503</v>
       </c>
@@ -3004,7 +2969,7 @@
         <v>56900307</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A19" s="6">
         <v>103022803</v>
       </c>
@@ -3045,7 +3010,7 @@
         <v>253404913</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A20" s="6">
         <v>103023153</v>
       </c>
@@ -3086,7 +3051,7 @@
         <v>473412241</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A21" s="6">
         <v>103023912</v>
       </c>
@@ -3127,7 +3092,7 @@
         <v>2022280386</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A22" s="6">
         <v>103024102</v>
       </c>
@@ -3168,7 +3133,7 @@
         <v>816406135</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A23" s="6">
         <v>103024603</v>
       </c>
@@ -3209,7 +3174,7 @@
         <v>965102439</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A24" s="6">
         <v>103024753</v>
       </c>
@@ -3250,7 +3215,7 @@
         <v>411141297</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A25" s="6">
         <v>103025002</v>
       </c>
@@ -3291,7 +3256,7 @@
         <v>679959375</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A26" s="6">
         <v>103026002</v>
       </c>
@@ -3332,7 +3297,7 @@
         <v>461285597</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A27" s="6">
         <v>103026303</v>
       </c>
@@ -3373,7 +3338,7 @@
         <v>1183865379</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A28" s="6">
         <v>103026343</v>
       </c>
@@ -3414,7 +3379,7 @@
         <v>1109757254</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A29" s="6">
         <v>103026402</v>
       </c>
@@ -3455,7 +3420,7 @@
         <v>1866103227</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A30" s="6">
         <v>103026852</v>
       </c>
@@ -3496,7 +3461,7 @@
         <v>3095297883</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A31" s="6">
         <v>103026902</v>
       </c>
@@ -3537,7 +3502,7 @@
         <v>1396045862</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A32" s="6">
         <v>103026873</v>
       </c>
@@ -3578,7 +3543,7 @@
         <v>321859027</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A33" s="6">
         <v>103027352</v>
       </c>
@@ -3619,7 +3584,7 @@
         <v>823515690</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A34" s="6">
         <v>103021003</v>
       </c>
@@ -3660,7 +3625,7 @@
         <v>1819960281</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A35" s="6">
         <v>102027451</v>
       </c>
@@ -3701,7 +3666,7 @@
         <v>8689448212</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A36" s="6">
         <v>103027503</v>
       </c>
@@ -3742,7 +3707,7 @@
         <v>840874109</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A37" s="6">
         <v>103027753</v>
       </c>
@@ -3783,7 +3748,7 @@
         <v>1182117677</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A38" s="6">
         <v>103028203</v>
       </c>
@@ -3824,7 +3789,7 @@
         <v>337581788</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A39" s="6">
         <v>103028302</v>
       </c>
@@ -3865,7 +3830,7 @@
         <v>1131077153</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A40" s="6">
         <v>103028653</v>
       </c>
@@ -3906,7 +3871,7 @@
         <v>197009185</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A41" s="6">
         <v>103028703</v>
       </c>
@@ -3947,7 +3912,7 @@
         <v>820726387</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A42" s="6">
         <v>103028753</v>
       </c>
@@ -3988,7 +3953,7 @@
         <v>429706272</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A43" s="6">
         <v>103028833</v>
       </c>
@@ -4029,7 +3994,7 @@
         <v>310631865</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A44" s="6">
         <v>103028853</v>
       </c>
@@ -4070,7 +4035,7 @@
         <v>159310310</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A45" s="6">
         <v>103029203</v>
       </c>
@@ -4111,7 +4076,7 @@
         <v>1406489978</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A46" s="6">
         <v>103029403</v>
       </c>
@@ -4152,7 +4117,7 @@
         <v>833820739</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A47" s="6">
         <v>103029553</v>
       </c>
@@ -4193,7 +4158,7 @@
         <v>729415432</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A48" s="6">
         <v>103029603</v>
       </c>
@@ -4234,7 +4199,7 @@
         <v>440241518</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A49" s="6">
         <v>103029803</v>
       </c>
@@ -4275,7 +4240,7 @@
         <v>288452338</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A50" s="6">
         <v>103029902</v>
       </c>
@@ -4316,7 +4281,7 @@
         <v>1102487910</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A51" s="6">
         <v>128030603</v>
       </c>
@@ -4357,7 +4322,7 @@
         <v>175770311</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A52" s="6">
         <v>128030852</v>
       </c>
@@ -4398,7 +4363,7 @@
         <v>876383427</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A53" s="6">
         <v>128033053</v>
       </c>
@@ -4439,7 +4404,7 @@
         <v>412335189</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A54" s="6">
         <v>128034503</v>
       </c>
@@ -4480,7 +4445,7 @@
         <v>122977981</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A55" s="6">
         <v>127040503</v>
       </c>
@@ -4521,7 +4486,7 @@
         <v>136490925</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A56" s="6">
         <v>127040703</v>
       </c>
@@ -4562,7 +4527,7 @@
         <v>576019698</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A57" s="6">
         <v>127041203</v>
       </c>
@@ -4603,7 +4568,7 @@
         <v>470904516</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A58" s="6">
         <v>127041503</v>
       </c>
@@ -4644,7 +4609,7 @@
         <v>208505930</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A59" s="6">
         <v>127041603</v>
       </c>
@@ -4685,7 +4650,7 @@
         <v>742117178</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A60" s="6">
         <v>127042003</v>
       </c>
@@ -4726,7 +4691,7 @@
         <v>525445663</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A61" s="6">
         <v>127042853</v>
       </c>
@@ -4767,7 +4732,7 @@
         <v>249215654</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A62" s="6">
         <v>127044103</v>
       </c>
@@ -4808,7 +4773,7 @@
         <v>503897973</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A63" s="6">
         <v>127045303</v>
       </c>
@@ -4849,7 +4814,7 @@
         <v>40543429</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A64" s="6">
         <v>127045653</v>
       </c>
@@ -4890,7 +4855,7 @@
         <v>187701827</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A65" s="6">
         <v>127045853</v>
       </c>
@@ -4931,7 +4896,7 @@
         <v>277249520</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A66" s="6">
         <v>127046903</v>
       </c>
@@ -4972,7 +4937,7 @@
         <v>129717368</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A67" s="6">
         <v>127047404</v>
       </c>
@@ -5013,7 +4978,7 @@
         <v>187508859</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A68" s="6">
         <v>127049303</v>
       </c>
@@ -5054,7 +5019,7 @@
         <v>125862799</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A69" s="6">
         <v>108051003</v>
       </c>
@@ -5095,7 +5060,7 @@
         <v>356605597</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A70" s="6">
         <v>108051503</v>
       </c>
@@ -5136,7 +5101,7 @@
         <v>202260728</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A71" s="6">
         <v>108053003</v>
       </c>
@@ -5177,7 +5142,7 @@
         <v>178715073</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A72" s="6">
         <v>108056004</v>
       </c>
@@ -5218,7 +5183,7 @@
         <v>142157477</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A73" s="6">
         <v>108058003</v>
       </c>
@@ -5259,7 +5224,7 @@
         <v>114744036</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A74" s="6">
         <v>114060503</v>
       </c>
@@ -5300,7 +5265,7 @@
         <v>164773602</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A75" s="6">
         <v>114060753</v>
       </c>
@@ -5341,7 +5306,7 @@
         <v>1786725815</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A76" s="6">
         <v>114060853</v>
       </c>
@@ -5382,7 +5347,7 @@
         <v>358172397</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A77" s="6">
         <v>114061103</v>
       </c>
@@ -5423,7 +5388,7 @@
         <v>546482458</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A78" s="6">
         <v>114061503</v>
       </c>
@@ -5464,7 +5429,7 @@
         <v>732669441</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A79" s="6">
         <v>114062003</v>
       </c>
@@ -5505,7 +5470,7 @@
         <v>874465227</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A80" s="6">
         <v>114062503</v>
       </c>
@@ -5546,7 +5511,7 @@
         <v>549588044</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A81" s="6">
         <v>114063003</v>
       </c>
@@ -5587,7 +5552,7 @@
         <v>1082487334</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A82" s="6">
         <v>114063503</v>
       </c>
@@ -5628,7 +5593,7 @@
         <v>477161666</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A83" s="6">
         <v>114064003</v>
       </c>
@@ -5669,7 +5634,7 @@
         <v>396261293</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A84" s="6">
         <v>114065503</v>
       </c>
@@ -5710,7 +5675,7 @@
         <v>600387781</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A85" s="6">
         <v>114066503</v>
       </c>
@@ -5751,7 +5716,7 @@
         <v>432248256</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A86" s="6">
         <v>114067002</v>
       </c>
@@ -5792,7 +5757,7 @@
         <v>1073037060</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A87" s="6">
         <v>114067503</v>
       </c>
@@ -5833,7 +5798,7 @@
         <v>463838682</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A88" s="6">
         <v>114068003</v>
       </c>
@@ -5874,7 +5839,7 @@
         <v>354250968</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A89" s="6">
         <v>114068103</v>
       </c>
@@ -5915,7 +5880,7 @@
         <v>804439411</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A90" s="6">
         <v>114069103</v>
       </c>
@@ -5956,7 +5921,7 @@
         <v>1466956976</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A91" s="6">
         <v>114069353</v>
       </c>
@@ -5997,7 +5962,7 @@
         <v>669724980</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A92" s="6">
         <v>108070502</v>
       </c>
@@ -6038,7 +6003,7 @@
         <v>1092590743</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A93" s="6">
         <v>108071003</v>
       </c>
@@ -6079,7 +6044,7 @@
         <v>222536401</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A94" s="6">
         <v>108071504</v>
       </c>
@@ -6120,7 +6085,7 @@
         <v>117271491</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A95" s="6">
         <v>108073503</v>
       </c>
@@ -6161,7 +6126,7 @@
         <v>889968313</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A96" s="6">
         <v>108077503</v>
       </c>
@@ -6202,7 +6167,7 @@
         <v>294668423</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A97" s="6">
         <v>108078003</v>
       </c>
@@ -6243,7 +6208,7 @@
         <v>279727368</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A98" s="6">
         <v>108079004</v>
       </c>
@@ -6284,7 +6249,7 @@
         <v>67603485</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A99" s="6">
         <v>117080503</v>
       </c>
@@ -6325,7 +6290,7 @@
         <v>278165714</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A100" s="6">
         <v>117081003</v>
       </c>
@@ -6366,7 +6331,7 @@
         <v>109546000</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A101" s="6">
         <v>117083004</v>
       </c>
@@ -6407,7 +6372,7 @@
         <v>100607591</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A102" s="6">
         <v>117086003</v>
       </c>
@@ -6448,7 +6413,7 @@
         <v>136835816</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A103" s="6">
         <v>117086503</v>
       </c>
@@ -6489,7 +6454,7 @@
         <v>210965631</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A104" s="6">
         <v>117086653</v>
       </c>
@@ -6530,7 +6495,7 @@
         <v>179683992</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A105" s="6">
         <v>117089003</v>
       </c>
@@ -6571,7 +6536,7 @@
         <v>215830619</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A106" s="6">
         <v>122091002</v>
       </c>
@@ -6612,7 +6577,7 @@
         <v>1813256635</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A107" s="6">
         <v>122091303</v>
       </c>
@@ -6653,7 +6618,7 @@
         <v>203600922</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A108" s="6">
         <v>122091352</v>
       </c>
@@ -6694,7 +6659,7 @@
         <v>1233249510</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A109" s="6">
         <v>122092002</v>
       </c>
@@ -6735,7 +6700,7 @@
         <v>1711218978</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A110" s="6">
         <v>122092102</v>
       </c>
@@ -6776,7 +6741,7 @@
         <v>6709300946</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A111" s="6">
         <v>122092353</v>
       </c>
@@ -6817,7 +6782,7 @@
         <v>5124435109</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A112" s="6">
         <v>122097203</v>
       </c>
@@ -6858,7 +6823,7 @@
         <v>297455913</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A113" s="6">
         <v>122097502</v>
       </c>
@@ -6899,7 +6864,7 @@
         <v>2508686269</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A114" s="6">
         <v>122097604</v>
       </c>
@@ -6940,7 +6905,7 @@
         <v>1411084486</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A115" s="6">
         <v>122098003</v>
       </c>
@@ -6981,7 +6946,7 @@
         <v>731300678</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A116" s="6">
         <v>122098103</v>
       </c>
@@ -7022,7 +6987,7 @@
         <v>2072256989</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A117" s="6">
         <v>122098202</v>
       </c>
@@ -7063,7 +7028,7 @@
         <v>3495552004</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A118" s="6">
         <v>122098403</v>
       </c>
@@ -7104,7 +7069,7 @@
         <v>1199215732</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A119" s="6">
         <v>104101252</v>
       </c>
@@ -7145,7 +7110,7 @@
         <v>1324191424</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A120" s="6">
         <v>104103603</v>
       </c>
@@ -7186,12 +7151,12 @@
         <v>201972274</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A121" s="6">
         <v>104107803</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C121" s="7" t="s">
         <v>107</v>
@@ -7227,7 +7192,7 @@
         <v>576599456</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A122" s="6">
         <v>104105003</v>
       </c>
@@ -7268,7 +7233,7 @@
         <v>1260047425</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A123" s="6">
         <v>104105353</v>
       </c>
@@ -7309,7 +7274,7 @@
         <v>189979511</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A124" s="6">
         <v>104107903</v>
       </c>
@@ -7350,7 +7315,7 @@
         <v>2373027886</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A125" s="6">
         <v>104107503</v>
       </c>
@@ -7391,7 +7356,7 @@
         <v>398995674</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A126" s="6">
         <v>108110603</v>
       </c>
@@ -7432,7 +7397,7 @@
         <v>82881011</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A127" s="6">
         <v>108111203</v>
       </c>
@@ -7473,7 +7438,7 @@
         <v>207296567</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A128" s="6">
         <v>108111303</v>
       </c>
@@ -7514,7 +7479,7 @@
         <v>309964153</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A129" s="6">
         <v>108111403</v>
       </c>
@@ -7555,7 +7520,7 @@
         <v>118294097</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A130" s="6">
         <v>108112003</v>
       </c>
@@ -7596,7 +7561,7 @@
         <v>72626673</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A131" s="6">
         <v>108112203</v>
       </c>
@@ -7637,7 +7602,7 @@
         <v>286822772</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A132" s="6">
         <v>108112502</v>
       </c>
@@ -7678,7 +7643,7 @@
         <v>295507036</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A133" s="6">
         <v>108114503</v>
       </c>
@@ -7719,7 +7684,7 @@
         <v>154219952</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A134" s="6">
         <v>108116003</v>
       </c>
@@ -7760,7 +7725,7 @@
         <v>274872161</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A135" s="6">
         <v>108116303</v>
       </c>
@@ -7801,7 +7766,7 @@
         <v>111973339</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A136" s="6">
         <v>108116503</v>
       </c>
@@ -7842,7 +7807,7 @@
         <v>342559139</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A137" s="6">
         <v>108118503</v>
       </c>
@@ -7883,7 +7848,7 @@
         <v>351059313</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A138" s="6">
         <v>109122703</v>
       </c>
@@ -7924,7 +7889,7 @@
         <v>73430685</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A139" s="6">
         <v>121135003</v>
       </c>
@@ -7965,7 +7930,7 @@
         <v>355726608</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A140" s="6">
         <v>121135503</v>
       </c>
@@ -8006,7 +7971,7 @@
         <v>388960604</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A141" s="6">
         <v>121136503</v>
       </c>
@@ -8047,7 +8012,7 @@
         <v>345851348</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A142" s="6">
         <v>121136603</v>
       </c>
@@ -8088,7 +8053,7 @@
         <v>200145373</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A143" s="6">
         <v>121139004</v>
       </c>
@@ -8129,7 +8094,7 @@
         <v>104117629</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A144" s="6">
         <v>110141003</v>
       </c>
@@ -8170,7 +8135,7 @@
         <v>287233219</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A145" s="6">
         <v>110141103</v>
       </c>
@@ -8211,7 +8176,7 @@
         <v>645248811</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A146" s="6">
         <v>110147003</v>
       </c>
@@ -8252,7 +8217,7 @@
         <v>296355262</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A147" s="6">
         <v>110148002</v>
       </c>
@@ -8293,7 +8258,7 @@
         <v>2369132610</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A148" s="6">
         <v>124150503</v>
       </c>
@@ -8334,7 +8299,7 @@
         <v>1077871156</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A149" s="6">
         <v>124151902</v>
       </c>
@@ -8375,7 +8340,7 @@
         <v>1783710194</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A150" s="6">
         <v>124152003</v>
       </c>
@@ -8416,7 +8381,7 @@
         <v>4230982727</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A151" s="6">
         <v>124153503</v>
       </c>
@@ -8457,7 +8422,7 @@
         <v>2650005676</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A152" s="6">
         <v>124154003</v>
       </c>
@@ -8498,7 +8463,7 @@
         <v>980308094</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A153" s="6">
         <v>124156503</v>
       </c>
@@ -8539,7 +8504,7 @@
         <v>605813894</v>
       </c>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A154" s="6">
         <v>124156603</v>
       </c>
@@ -8580,7 +8545,7 @@
         <v>2034676345</v>
       </c>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A155" s="6">
         <v>124156703</v>
       </c>
@@ -8621,7 +8586,7 @@
         <v>610919739</v>
       </c>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A156" s="6">
         <v>124157203</v>
       </c>
@@ -8662,7 +8627,7 @@
         <v>1752161263</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A157" s="6">
         <v>124157802</v>
       </c>
@@ -8703,7 +8668,7 @@
         <v>4250427193</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A158" s="6">
         <v>124158503</v>
       </c>
@@ -8744,7 +8709,7 @@
         <v>1768828691</v>
       </c>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A159" s="6">
         <v>124159002</v>
       </c>
@@ -8785,7 +8750,7 @@
         <v>5524523899</v>
       </c>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A160" s="6">
         <v>106160303</v>
       </c>
@@ -8826,7 +8791,7 @@
         <v>108102125</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A161" s="6">
         <v>106161203</v>
       </c>
@@ -8867,7 +8832,7 @@
         <v>152284190</v>
       </c>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A162" s="6">
         <v>106161703</v>
       </c>
@@ -8908,7 +8873,7 @@
         <v>141269962</v>
       </c>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A163" s="6">
         <v>106166503</v>
       </c>
@@ -8949,7 +8914,7 @@
         <v>158854301</v>
       </c>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A164" s="6">
         <v>106167504</v>
       </c>
@@ -8990,7 +8955,7 @@
         <v>97779457</v>
       </c>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A165" s="6">
         <v>106168003</v>
       </c>
@@ -9031,7 +8996,7 @@
         <v>150974391</v>
       </c>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A166" s="6">
         <v>106169003</v>
       </c>
@@ -9072,7 +9037,7 @@
         <v>66410329</v>
       </c>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A167" s="6">
         <v>110171003</v>
       </c>
@@ -9113,7 +9078,7 @@
         <v>344446859</v>
       </c>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A168" s="6">
         <v>110171803</v>
       </c>
@@ -9154,7 +9119,7 @@
         <v>140633502</v>
       </c>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A169" s="6">
         <v>106172003</v>
       </c>
@@ -9195,7 +9160,7 @@
         <v>703695728</v>
       </c>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A170" s="6">
         <v>110173003</v>
       </c>
@@ -9236,7 +9201,7 @@
         <v>92955091</v>
       </c>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A171" s="6">
         <v>110173504</v>
       </c>
@@ -9277,7 +9242,7 @@
         <v>39939921</v>
       </c>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A172" s="6">
         <v>110175003</v>
       </c>
@@ -9318,7 +9283,7 @@
         <v>124979442</v>
       </c>
     </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A173" s="6">
         <v>110177003</v>
       </c>
@@ -9359,7 +9324,7 @@
         <v>275680014</v>
       </c>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A174" s="6">
         <v>110179003</v>
       </c>
@@ -9400,7 +9365,7 @@
         <v>150363265</v>
       </c>
     </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A175" s="6">
         <v>110183602</v>
       </c>
@@ -9441,7 +9406,7 @@
         <v>725330397</v>
       </c>
     </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A176" s="6">
         <v>116191004</v>
       </c>
@@ -9482,7 +9447,7 @@
         <v>118205598</v>
       </c>
     </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A177" s="6">
         <v>116191103</v>
       </c>
@@ -9523,7 +9488,7 @@
         <v>434550621</v>
       </c>
     </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A178" s="6">
         <v>116191203</v>
       </c>
@@ -9564,7 +9529,7 @@
         <v>330064186</v>
       </c>
     </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A179" s="6">
         <v>116191503</v>
       </c>
@@ -9605,7 +9570,7 @@
         <v>419790590</v>
       </c>
     </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A180" s="6">
         <v>116195004</v>
       </c>
@@ -9646,7 +9611,7 @@
         <v>115607815</v>
       </c>
     </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A181" s="6">
         <v>116197503</v>
       </c>
@@ -9687,7 +9652,7 @@
         <v>296827456</v>
       </c>
     </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A182" s="6">
         <v>105201033</v>
       </c>
@@ -9728,7 +9693,7 @@
         <v>337750367</v>
       </c>
     </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A183" s="6">
         <v>105201352</v>
       </c>
@@ -9769,7 +9734,7 @@
         <v>578536833</v>
       </c>
     </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A184" s="6">
         <v>105204703</v>
       </c>
@@ -9810,7 +9775,7 @@
         <v>458252478</v>
       </c>
     </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A185" s="6">
         <v>115210503</v>
       </c>
@@ -9851,7 +9816,7 @@
         <v>513133770</v>
       </c>
     </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A186" s="6">
         <v>115211003</v>
       </c>
@@ -9892,7 +9857,7 @@
         <v>427562911</v>
       </c>
     </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A187" s="6">
         <v>115211103</v>
       </c>
@@ -9933,7 +9898,7 @@
         <v>941214744</v>
       </c>
     </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A188" s="6">
         <v>115211603</v>
       </c>
@@ -9974,7 +9939,7 @@
         <v>2640875144</v>
       </c>
     </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A189" s="6">
         <v>115212503</v>
       </c>
@@ -10015,7 +9980,7 @@
         <v>573383937</v>
       </c>
     </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A190" s="6">
         <v>115216503</v>
       </c>
@@ -10056,7 +10021,7 @@
         <v>1337881462</v>
       </c>
     </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A191" s="6">
         <v>115218003</v>
       </c>
@@ -10097,7 +10062,7 @@
         <v>610925260</v>
       </c>
     </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A192" s="6">
         <v>115218303</v>
       </c>
@@ -10138,7 +10103,7 @@
         <v>511537563</v>
       </c>
     </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A193" s="6">
         <v>115221402</v>
       </c>
@@ -10179,7 +10144,7 @@
         <v>3025356751</v>
       </c>
     </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A194" s="6">
         <v>115221753</v>
       </c>
@@ -10220,7 +10185,7 @@
         <v>1183426699</v>
       </c>
     </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A195" s="6">
         <v>115222504</v>
       </c>
@@ -10261,7 +10226,7 @@
         <v>199807565</v>
       </c>
     </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A196" s="6">
         <v>115222752</v>
       </c>
@@ -10302,7 +10267,7 @@
         <v>728015174</v>
       </c>
     </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A197" s="6">
         <v>115224003</v>
       </c>
@@ -10343,7 +10308,7 @@
         <v>950087830</v>
       </c>
     </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A198" s="6">
         <v>115226003</v>
       </c>
@@ -10384,7 +10349,7 @@
         <v>442922344</v>
       </c>
     </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A199" s="6">
         <v>115226103</v>
       </c>
@@ -10425,7 +10390,7 @@
         <v>165211929</v>
       </c>
     </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A200" s="6">
         <v>115228003</v>
       </c>
@@ -10466,7 +10431,7 @@
         <v>122319194</v>
       </c>
     </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A201" s="6">
         <v>115228303</v>
       </c>
@@ -10507,7 +10472,7 @@
         <v>739983753</v>
       </c>
     </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A202" s="6">
         <v>115229003</v>
       </c>
@@ -10548,7 +10513,7 @@
         <v>199351343</v>
       </c>
     </row>
-    <row r="203" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A203" s="6">
         <v>125231232</v>
       </c>
@@ -10589,7 +10554,7 @@
         <v>439530731</v>
       </c>
     </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A204" s="6">
         <v>125231303</v>
       </c>
@@ -10630,7 +10595,7 @@
         <v>516150688</v>
       </c>
     </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A205" s="6">
         <v>125234103</v>
       </c>
@@ -10671,7 +10636,7 @@
         <v>1347090167</v>
       </c>
     </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A206" s="6">
         <v>125234502</v>
       </c>
@@ -10712,7 +10677,7 @@
         <v>2469728443</v>
       </c>
     </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A207" s="6">
         <v>125235103</v>
       </c>
@@ -10753,7 +10718,7 @@
         <v>581991285</v>
       </c>
     </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A208" s="6">
         <v>125235502</v>
       </c>
@@ -10794,7 +10759,7 @@
         <v>2338949823</v>
       </c>
     </row>
-    <row r="209" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A209" s="6">
         <v>125236903</v>
       </c>
@@ -10835,7 +10800,7 @@
         <v>759887864</v>
       </c>
     </row>
-    <row r="210" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A210" s="6">
         <v>125237603</v>
       </c>
@@ -10876,7 +10841,7 @@
         <v>2783814852</v>
       </c>
     </row>
-    <row r="211" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A211" s="6">
         <v>125237702</v>
       </c>
@@ -10917,7 +10882,7 @@
         <v>1070947346</v>
       </c>
     </row>
-    <row r="212" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A212" s="6">
         <v>125237903</v>
       </c>
@@ -10958,7 +10923,7 @@
         <v>2038787009</v>
       </c>
     </row>
-    <row r="213" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A213" s="6">
         <v>125238402</v>
       </c>
@@ -10999,7 +10964,7 @@
         <v>479337657</v>
       </c>
     </row>
-    <row r="214" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A214" s="6">
         <v>125238502</v>
       </c>
@@ -11040,7 +11005,7 @@
         <v>1067904363</v>
       </c>
     </row>
-    <row r="215" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A215" s="6">
         <v>125239452</v>
       </c>
@@ -11081,7 +11046,7 @@
         <v>2000260922</v>
       </c>
     </row>
-    <row r="216" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A216" s="6">
         <v>125239603</v>
       </c>
@@ -11122,7 +11087,7 @@
         <v>1125757460</v>
       </c>
     </row>
-    <row r="217" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A217" s="6">
         <v>125239652</v>
       </c>
@@ -11163,7 +11128,7 @@
         <v>854683956</v>
       </c>
     </row>
-    <row r="218" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A218" s="6">
         <v>109243503</v>
       </c>
@@ -11204,7 +11169,7 @@
         <v>83251187</v>
       </c>
     </row>
-    <row r="219" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A219" s="6">
         <v>109246003</v>
       </c>
@@ -11245,7 +11210,7 @@
         <v>139731042</v>
       </c>
     </row>
-    <row r="220" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A220" s="6">
         <v>109248003</v>
       </c>
@@ -11286,7 +11251,7 @@
         <v>437968584</v>
       </c>
     </row>
-    <row r="221" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A221" s="6">
         <v>105251453</v>
       </c>
@@ -11327,7 +11292,7 @@
         <v>219989186</v>
       </c>
     </row>
-    <row r="222" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A222" s="6">
         <v>105252602</v>
       </c>
@@ -11368,7 +11333,7 @@
         <v>1435681235</v>
       </c>
     </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A223" s="6">
         <v>105253303</v>
       </c>
@@ -11409,7 +11374,7 @@
         <v>439687084</v>
       </c>
     </row>
-    <row r="224" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A224" s="6">
         <v>105253553</v>
       </c>
@@ -11450,7 +11415,7 @@
         <v>341173031</v>
       </c>
     </row>
-    <row r="225" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A225" s="6">
         <v>105253903</v>
       </c>
@@ -11491,7 +11456,7 @@
         <v>372592918</v>
       </c>
     </row>
-    <row r="226" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A226" s="6">
         <v>105254053</v>
       </c>
@@ -11532,7 +11497,7 @@
         <v>220394242</v>
       </c>
     </row>
-    <row r="227" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A227" s="6">
         <v>105254353</v>
       </c>
@@ -11573,7 +11538,7 @@
         <v>358344035</v>
       </c>
     </row>
-    <row r="228" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A228" s="6">
         <v>105256553</v>
       </c>
@@ -11614,7 +11579,7 @@
         <v>115876363</v>
       </c>
     </row>
-    <row r="229" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A229" s="6">
         <v>105257602</v>
       </c>
@@ -11655,7 +11620,7 @@
         <v>1862670647</v>
       </c>
     </row>
-    <row r="230" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A230" s="6">
         <v>105258303</v>
       </c>
@@ -11696,7 +11661,7 @@
         <v>241067818</v>
       </c>
     </row>
-    <row r="231" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A231" s="6">
         <v>105258503</v>
       </c>
@@ -11737,7 +11702,7 @@
         <v>171619184</v>
       </c>
     </row>
-    <row r="232" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A232" s="6">
         <v>105259103</v>
       </c>
@@ -11778,7 +11743,7 @@
         <v>111493849</v>
       </c>
     </row>
-    <row r="233" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A233" s="6">
         <v>105259703</v>
       </c>
@@ -11819,7 +11784,7 @@
         <v>230788373</v>
       </c>
     </row>
-    <row r="234" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A234" s="6">
         <v>101260303</v>
       </c>
@@ -11860,7 +11825,7 @@
         <v>420777807</v>
       </c>
     </row>
-    <row r="235" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A235" s="6">
         <v>101260803</v>
       </c>
@@ -11901,7 +11866,7 @@
         <v>197860665</v>
       </c>
     </row>
-    <row r="236" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A236" s="6">
         <v>101261302</v>
       </c>
@@ -11942,7 +11907,7 @@
         <v>629783957</v>
       </c>
     </row>
-    <row r="237" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A237" s="6">
         <v>101262903</v>
       </c>
@@ -11983,7 +11948,7 @@
         <v>168963987</v>
       </c>
     </row>
-    <row r="238" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A238" s="6">
         <v>101264003</v>
       </c>
@@ -12024,7 +11989,7 @@
         <v>472089679</v>
       </c>
     </row>
-    <row r="239" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A239" s="6">
         <v>101268003</v>
       </c>
@@ -12065,7 +12030,7 @@
         <v>441057753</v>
       </c>
     </row>
-    <row r="240" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A240" s="6">
         <v>106272003</v>
       </c>
@@ -12106,7 +12071,7 @@
         <v>74184782</v>
       </c>
     </row>
-    <row r="241" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A241" s="6">
         <v>112281302</v>
       </c>
@@ -12147,7 +12112,7 @@
         <v>1715788905</v>
       </c>
     </row>
-    <row r="242" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A242" s="6">
         <v>112282004</v>
       </c>
@@ -12188,7 +12153,7 @@
         <v>94549050</v>
       </c>
     </row>
-    <row r="243" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A243" s="6">
         <v>112283003</v>
       </c>
@@ -12229,7 +12194,7 @@
         <v>577129882</v>
       </c>
     </row>
-    <row r="244" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A244" s="6">
         <v>112286003</v>
       </c>
@@ -12270,7 +12235,7 @@
         <v>442393538</v>
       </c>
     </row>
-    <row r="245" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A245" s="6">
         <v>112289003</v>
       </c>
@@ -12311,7 +12276,7 @@
         <v>748325394</v>
       </c>
     </row>
-    <row r="246" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A246" s="6">
         <v>111291304</v>
       </c>
@@ -12352,7 +12317,7 @@
         <v>137146487</v>
       </c>
     </row>
-    <row r="247" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A247" s="6">
         <v>111292304</v>
       </c>
@@ -12393,7 +12358,7 @@
         <v>57866030</v>
       </c>
     </row>
-    <row r="248" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A248" s="6">
         <v>111297504</v>
       </c>
@@ -12434,7 +12399,7 @@
         <v>118749662</v>
       </c>
     </row>
-    <row r="249" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A249" s="6">
         <v>101301303</v>
       </c>
@@ -12475,7 +12440,7 @@
         <v>132513798</v>
       </c>
     </row>
-    <row r="250" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A250" s="6">
         <v>101301403</v>
       </c>
@@ -12516,7 +12481,7 @@
         <v>302165402</v>
       </c>
     </row>
-    <row r="251" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A251" s="6">
         <v>101303503</v>
       </c>
@@ -12557,7 +12522,7 @@
         <v>111495398</v>
       </c>
     </row>
-    <row r="252" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A252" s="6">
         <v>101306503</v>
       </c>
@@ -12598,7 +12563,7 @@
         <v>104772852</v>
       </c>
     </row>
-    <row r="253" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A253" s="6">
         <v>101308503</v>
       </c>
@@ -12639,7 +12604,7 @@
         <v>136542730</v>
       </c>
     </row>
-    <row r="254" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A254" s="6">
         <v>111312503</v>
       </c>
@@ -12680,7 +12645,7 @@
         <v>323653246</v>
       </c>
     </row>
-    <row r="255" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A255" s="6">
         <v>111312804</v>
       </c>
@@ -12721,7 +12686,7 @@
         <v>103796290</v>
       </c>
     </row>
-    <row r="256" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A256" s="6">
         <v>111316003</v>
       </c>
@@ -12762,7 +12727,7 @@
         <v>151921497</v>
       </c>
     </row>
-    <row r="257" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A257" s="6">
         <v>111317503</v>
       </c>
@@ -12803,7 +12768,7 @@
         <v>153117699</v>
       </c>
     </row>
-    <row r="258" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A258" s="6">
         <v>128323303</v>
       </c>
@@ -12844,7 +12809,7 @@
         <v>120250248</v>
       </c>
     </row>
-    <row r="259" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A259" s="6">
         <v>128323703</v>
       </c>
@@ -12885,7 +12850,7 @@
         <v>582459547</v>
       </c>
     </row>
-    <row r="260" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A260" s="6">
         <v>128325203</v>
       </c>
@@ -12926,7 +12891,7 @@
         <v>188736313</v>
       </c>
     </row>
-    <row r="261" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A261" s="6">
         <v>128326303</v>
       </c>
@@ -12967,7 +12932,7 @@
         <v>107435955</v>
       </c>
     </row>
-    <row r="262" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A262" s="6">
         <v>128327303</v>
       </c>
@@ -13008,12 +12973,12 @@
         <v>107625672</v>
       </c>
     </row>
-    <row r="263" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A263" s="6">
         <v>128321103</v>
       </c>
       <c r="B263" s="7" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C263" s="7" t="s">
         <v>232</v>
@@ -13049,7 +13014,7 @@
         <v>268720994</v>
       </c>
     </row>
-    <row r="264" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A264" s="6">
         <v>128328003</v>
       </c>
@@ -13090,7 +13055,7 @@
         <v>140160526</v>
       </c>
     </row>
-    <row r="265" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A265" s="6">
         <v>106330703</v>
       </c>
@@ -13131,7 +13096,7 @@
         <v>160342314</v>
       </c>
     </row>
-    <row r="266" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A266" s="6">
         <v>106330803</v>
       </c>
@@ -13172,7 +13137,7 @@
         <v>236669307</v>
       </c>
     </row>
-    <row r="267" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A267" s="6">
         <v>106338003</v>
       </c>
@@ -13213,7 +13178,7 @@
         <v>389142081</v>
       </c>
     </row>
-    <row r="268" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A268" s="6">
         <v>111343603</v>
       </c>
@@ -13254,7 +13219,7 @@
         <v>488867988</v>
       </c>
     </row>
-    <row r="269" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A269" s="6">
         <v>119350303</v>
       </c>
@@ -13295,7 +13260,7 @@
         <v>1039324250</v>
       </c>
     </row>
-    <row r="270" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A270" s="6">
         <v>119351303</v>
       </c>
@@ -13336,7 +13301,7 @@
         <v>181072793</v>
       </c>
     </row>
-    <row r="271" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A271" s="6">
         <v>119352203</v>
       </c>
@@ -13377,7 +13342,7 @@
         <v>370894253</v>
       </c>
     </row>
-    <row r="272" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A272" s="6">
         <v>119354603</v>
       </c>
@@ -13418,7 +13383,7 @@
         <v>344284026</v>
       </c>
     </row>
-    <row r="273" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A273" s="6">
         <v>119355503</v>
       </c>
@@ -13459,7 +13424,7 @@
         <v>337391131</v>
       </c>
     </row>
-    <row r="274" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A274" s="6">
         <v>119356503</v>
       </c>
@@ -13500,7 +13465,7 @@
         <v>622798994</v>
       </c>
     </row>
-    <row r="275" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A275" s="6">
         <v>119356603</v>
       </c>
@@ -13541,7 +13506,7 @@
         <v>216758065</v>
       </c>
     </row>
-    <row r="276" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A276" s="6">
         <v>119357003</v>
       </c>
@@ -13582,7 +13547,7 @@
         <v>332343890</v>
       </c>
     </row>
-    <row r="277" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A277" s="6">
         <v>119357402</v>
       </c>
@@ -13623,7 +13588,7 @@
         <v>1172334546</v>
       </c>
     </row>
-    <row r="278" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A278" s="6">
         <v>119358403</v>
       </c>
@@ -13664,7 +13629,7 @@
         <v>483709302</v>
       </c>
     </row>
-    <row r="279" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A279" s="6">
         <v>113361303</v>
       </c>
@@ -13705,7 +13670,7 @@
         <v>750244886</v>
       </c>
     </row>
-    <row r="280" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A280" s="6">
         <v>113361503</v>
       </c>
@@ -13746,7 +13711,7 @@
         <v>198444007</v>
       </c>
     </row>
-    <row r="281" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A281" s="6">
         <v>113361703</v>
       </c>
@@ -13787,7 +13752,7 @@
         <v>1033861322</v>
       </c>
     </row>
-    <row r="282" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A282" s="6">
         <v>113362203</v>
       </c>
@@ -13828,7 +13793,7 @@
         <v>612651515</v>
       </c>
     </row>
-    <row r="283" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A283" s="6">
         <v>113362303</v>
       </c>
@@ -13869,7 +13834,7 @@
         <v>984220484</v>
       </c>
     </row>
-    <row r="284" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A284" s="6">
         <v>113362403</v>
       </c>
@@ -13910,7 +13875,7 @@
         <v>932035209</v>
       </c>
     </row>
-    <row r="285" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A285" s="6">
         <v>113362603</v>
       </c>
@@ -13951,7 +13916,7 @@
         <v>1000453532</v>
       </c>
     </row>
-    <row r="286" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A286" s="6">
         <v>113363103</v>
       </c>
@@ -13992,7 +13957,7 @@
         <v>1754964245</v>
       </c>
     </row>
-    <row r="287" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A287" s="6">
         <v>113363603</v>
       </c>
@@ -14033,7 +13998,7 @@
         <v>864928225</v>
       </c>
     </row>
-    <row r="288" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A288" s="6">
         <v>113364002</v>
       </c>
@@ -14074,7 +14039,7 @@
         <v>1572665991</v>
       </c>
     </row>
-    <row r="289" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A289" s="6">
         <v>113364403</v>
       </c>
@@ -14115,7 +14080,7 @@
         <v>819088101</v>
       </c>
     </row>
-    <row r="290" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A290" s="6">
         <v>113364503</v>
       </c>
@@ -14156,7 +14121,7 @@
         <v>1981972095</v>
       </c>
     </row>
-    <row r="291" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A291" s="6">
         <v>113365203</v>
       </c>
@@ -14197,7 +14162,7 @@
         <v>1208508749</v>
       </c>
     </row>
-    <row r="292" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A292" s="6">
         <v>113365303</v>
       </c>
@@ -14238,7 +14203,7 @@
         <v>584535717</v>
       </c>
     </row>
-    <row r="293" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A293" s="6">
         <v>113367003</v>
       </c>
@@ -14279,7 +14244,7 @@
         <v>717545242</v>
       </c>
     </row>
-    <row r="294" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A294" s="6">
         <v>113369003</v>
       </c>
@@ -14320,7 +14285,7 @@
         <v>1475294326</v>
       </c>
     </row>
-    <row r="295" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A295" s="6">
         <v>104372003</v>
       </c>
@@ -14361,7 +14326,7 @@
         <v>289272491</v>
       </c>
     </row>
-    <row r="296" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A296" s="6">
         <v>104374003</v>
       </c>
@@ -14402,7 +14367,7 @@
         <v>190859425</v>
       </c>
     </row>
-    <row r="297" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A297" s="6">
         <v>104375003</v>
       </c>
@@ -14443,7 +14408,7 @@
         <v>239998033</v>
       </c>
     </row>
-    <row r="298" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A298" s="6">
         <v>104375203</v>
       </c>
@@ -14484,7 +14449,7 @@
         <v>326424742</v>
       </c>
     </row>
-    <row r="299" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A299" s="6">
         <v>104375302</v>
       </c>
@@ -14525,7 +14490,7 @@
         <v>315738517</v>
       </c>
     </row>
-    <row r="300" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A300" s="6">
         <v>104376203</v>
       </c>
@@ -14566,7 +14531,7 @@
         <v>190658693</v>
       </c>
     </row>
-    <row r="301" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A301" s="6">
         <v>104377003</v>
       </c>
@@ -14607,7 +14572,7 @@
         <v>98510605</v>
       </c>
     </row>
-    <row r="302" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A302" s="6">
         <v>104378003</v>
       </c>
@@ -14648,7 +14613,7 @@
         <v>238897521</v>
       </c>
     </row>
-    <row r="303" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A303" s="6">
         <v>113380303</v>
       </c>
@@ -14689,7 +14654,7 @@
         <v>318174364</v>
       </c>
     </row>
-    <row r="304" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A304" s="6">
         <v>113381303</v>
       </c>
@@ -14730,7 +14695,7 @@
         <v>1074937527</v>
       </c>
     </row>
-    <row r="305" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A305" s="6">
         <v>113382303</v>
       </c>
@@ -14771,7 +14736,7 @@
         <v>578410469</v>
       </c>
     </row>
-    <row r="306" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A306" s="6">
         <v>113384603</v>
       </c>
@@ -14812,7 +14777,7 @@
         <v>384666607</v>
       </c>
     </row>
-    <row r="307" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A307" s="6">
         <v>113385003</v>
       </c>
@@ -14853,7 +14818,7 @@
         <v>487844595</v>
       </c>
     </row>
-    <row r="308" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A308" s="6">
         <v>113385303</v>
       </c>
@@ -14894,7 +14859,7 @@
         <v>791297029</v>
       </c>
     </row>
-    <row r="309" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A309" s="6">
         <v>121390302</v>
       </c>
@@ -14935,7 +14900,7 @@
         <v>1917903753</v>
       </c>
     </row>
-    <row r="310" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A310" s="6">
         <v>121391303</v>
       </c>
@@ -14976,7 +14941,7 @@
         <v>233519895</v>
       </c>
     </row>
-    <row r="311" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A311" s="6">
         <v>121392303</v>
       </c>
@@ -15017,7 +14982,7 @@
         <v>2134962134</v>
       </c>
     </row>
-    <row r="312" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A312" s="6">
         <v>121394503</v>
       </c>
@@ -15058,7 +15023,7 @@
         <v>327113836</v>
       </c>
     </row>
-    <row r="313" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A313" s="6">
         <v>121394603</v>
       </c>
@@ -15099,7 +15064,7 @@
         <v>555247388</v>
       </c>
     </row>
-    <row r="314" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A314" s="6">
         <v>121395103</v>
       </c>
@@ -15140,7 +15105,7 @@
         <v>2726988378</v>
       </c>
     </row>
-    <row r="315" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A315" s="6">
         <v>121395603</v>
       </c>
@@ -15181,7 +15146,7 @@
         <v>503728124</v>
       </c>
     </row>
-    <row r="316" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A316" s="6">
         <v>121395703</v>
       </c>
@@ -15222,7 +15187,7 @@
         <v>1518779247</v>
       </c>
     </row>
-    <row r="317" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A317" s="6">
         <v>121397803</v>
       </c>
@@ -15263,7 +15228,7 @@
         <v>814581010</v>
       </c>
     </row>
-    <row r="318" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A318" s="6">
         <v>118401403</v>
       </c>
@@ -15304,7 +15269,7 @@
         <v>744980262</v>
       </c>
     </row>
-    <row r="319" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A319" s="6">
         <v>118401603</v>
       </c>
@@ -15345,7 +15310,7 @@
         <v>803507292</v>
       </c>
     </row>
-    <row r="320" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A320" s="6">
         <v>118402603</v>
       </c>
@@ -15386,7 +15351,7 @@
         <v>298099320</v>
       </c>
     </row>
-    <row r="321" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A321" s="6">
         <v>118403003</v>
       </c>
@@ -15427,7 +15392,7 @@
         <v>291369469</v>
       </c>
     </row>
-    <row r="322" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A322" s="6">
         <v>118403302</v>
       </c>
@@ -15468,7 +15433,7 @@
         <v>1511376216</v>
       </c>
     </row>
-    <row r="323" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A323" s="6">
         <v>118403903</v>
       </c>
@@ -15509,7 +15474,7 @@
         <v>466885368</v>
       </c>
     </row>
-    <row r="324" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A324" s="6">
         <v>118406003</v>
       </c>
@@ -15550,7 +15515,7 @@
         <v>185450063</v>
       </c>
     </row>
-    <row r="325" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A325" s="6">
         <v>118406602</v>
       </c>
@@ -15591,7 +15556,7 @@
         <v>649648422</v>
       </c>
     </row>
-    <row r="326" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A326" s="6">
         <v>118408852</v>
       </c>
@@ -15632,7 +15597,7 @@
         <v>1066474388</v>
       </c>
     </row>
-    <row r="327" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A327" s="6">
         <v>118409203</v>
       </c>
@@ -15673,7 +15638,7 @@
         <v>472045638</v>
       </c>
     </row>
-    <row r="328" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A328" s="6">
         <v>118409302</v>
       </c>
@@ -15714,7 +15679,7 @@
         <v>869287316</v>
       </c>
     </row>
-    <row r="329" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A329" s="6">
         <v>117412003</v>
       </c>
@@ -15755,7 +15720,7 @@
         <v>247347068</v>
       </c>
     </row>
-    <row r="330" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A330" s="6">
         <v>117414003</v>
       </c>
@@ -15796,7 +15761,7 @@
         <v>401246001</v>
       </c>
     </row>
-    <row r="331" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A331" s="6">
         <v>117414203</v>
       </c>
@@ -15837,7 +15802,7 @@
         <v>353308883</v>
       </c>
     </row>
-    <row r="332" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A332" s="6">
         <v>117415004</v>
       </c>
@@ -15878,7 +15843,7 @@
         <v>142861926</v>
       </c>
     </row>
-    <row r="333" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A333" s="6">
         <v>117415103</v>
       </c>
@@ -15919,7 +15884,7 @@
         <v>359374317</v>
       </c>
     </row>
-    <row r="334" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A334" s="6">
         <v>117415303</v>
       </c>
@@ -15960,7 +15925,7 @@
         <v>179639047</v>
       </c>
     </row>
-    <row r="335" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A335" s="6">
         <v>117416103</v>
       </c>
@@ -16001,7 +15966,7 @@
         <v>202900706</v>
       </c>
     </row>
-    <row r="336" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A336" s="6">
         <v>117417202</v>
       </c>
@@ -16042,7 +16007,7 @@
         <v>710224498</v>
       </c>
     </row>
-    <row r="337" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A337" s="6">
         <v>109420803</v>
       </c>
@@ -16083,7 +16048,7 @@
         <v>334704745</v>
       </c>
     </row>
-    <row r="338" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A338" s="6">
         <v>109422303</v>
       </c>
@@ -16124,7 +16089,7 @@
         <v>135320575</v>
       </c>
     </row>
-    <row r="339" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A339" s="6">
         <v>109426003</v>
       </c>
@@ -16165,7 +16130,7 @@
         <v>60716408</v>
       </c>
     </row>
-    <row r="340" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A340" s="6">
         <v>109426303</v>
       </c>
@@ -16206,7 +16171,7 @@
         <v>94119355</v>
       </c>
     </row>
-    <row r="341" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A341" s="6">
         <v>109427503</v>
       </c>
@@ -16247,7 +16212,7 @@
         <v>95831980</v>
       </c>
     </row>
-    <row r="342" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A342" s="6">
         <v>104431304</v>
       </c>
@@ -16288,7 +16253,7 @@
         <v>79835402</v>
       </c>
     </row>
-    <row r="343" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A343" s="6">
         <v>104432503</v>
       </c>
@@ -16329,7 +16294,7 @@
         <v>56334971</v>
       </c>
     </row>
-    <row r="344" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A344" s="6">
         <v>104432803</v>
       </c>
@@ -16370,7 +16335,7 @@
         <v>178994541</v>
       </c>
     </row>
-    <row r="345" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A345" s="6">
         <v>104432903</v>
       </c>
@@ -16411,7 +16376,7 @@
         <v>389391880</v>
       </c>
     </row>
-    <row r="346" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A346" s="6">
         <v>104433303</v>
       </c>
@@ -16452,7 +16417,7 @@
         <v>425087567</v>
       </c>
     </row>
-    <row r="347" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A347" s="6">
         <v>104433604</v>
       </c>
@@ -16493,7 +16458,7 @@
         <v>71929729</v>
       </c>
     </row>
-    <row r="348" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A348" s="6">
         <v>104433903</v>
       </c>
@@ -16534,7 +16499,7 @@
         <v>173413998</v>
       </c>
     </row>
-    <row r="349" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A349" s="6">
         <v>104435003</v>
       </c>
@@ -16575,7 +16540,7 @@
         <v>196023754</v>
       </c>
     </row>
-    <row r="350" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A350" s="6">
         <v>104435303</v>
       </c>
@@ -16616,7 +16581,7 @@
         <v>154307942</v>
       </c>
     </row>
-    <row r="351" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A351" s="6">
         <v>104435603</v>
       </c>
@@ -16657,7 +16622,7 @@
         <v>180104558</v>
       </c>
     </row>
-    <row r="352" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A352" s="6">
         <v>104435703</v>
       </c>
@@ -16698,7 +16663,7 @@
         <v>172411356</v>
       </c>
     </row>
-    <row r="353" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A353" s="6">
         <v>104437503</v>
       </c>
@@ -16739,7 +16704,7 @@
         <v>151370064</v>
       </c>
     </row>
-    <row r="354" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A354" s="6">
         <v>111444602</v>
       </c>
@@ -16780,7 +16745,7 @@
         <v>865345982</v>
       </c>
     </row>
-    <row r="355" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A355" s="6">
         <v>120452003</v>
       </c>
@@ -16821,7 +16786,7 @@
         <v>774065365</v>
       </c>
     </row>
-    <row r="356" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A356" s="6">
         <v>120455203</v>
       </c>
@@ -16862,7 +16827,7 @@
         <v>722065119</v>
       </c>
     </row>
-    <row r="357" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A357" s="6">
         <v>120455403</v>
       </c>
@@ -16903,7 +16868,7 @@
         <v>1167356299</v>
       </c>
     </row>
-    <row r="358" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A358" s="6">
         <v>120456003</v>
       </c>
@@ -16944,7 +16909,7 @@
         <v>813151786</v>
       </c>
     </row>
-    <row r="359" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A359" s="6">
         <v>123460302</v>
       </c>
@@ -16985,7 +16950,7 @@
         <v>2743145299</v>
       </c>
     </row>
-    <row r="360" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A360" s="6">
         <v>123460504</v>
       </c>
@@ -17026,7 +16991,7 @@
         <v>200152286</v>
       </c>
     </row>
-    <row r="361" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A361" s="6">
         <v>123461302</v>
       </c>
@@ -17067,7 +17032,7 @@
         <v>1273850292</v>
       </c>
     </row>
-    <row r="362" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A362" s="6">
         <v>123461602</v>
       </c>
@@ -17108,7 +17073,7 @@
         <v>2866802940</v>
       </c>
     </row>
-    <row r="363" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A363" s="6">
         <v>123463603</v>
       </c>
@@ -17149,7 +17114,7 @@
         <v>1748263577</v>
       </c>
     </row>
-    <row r="364" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A364" s="6">
         <v>123463803</v>
       </c>
@@ -17190,7 +17155,7 @@
         <v>204528483</v>
       </c>
     </row>
-    <row r="365" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A365" s="6">
         <v>123464502</v>
       </c>
@@ -17231,7 +17196,7 @@
         <v>8899879707</v>
       </c>
     </row>
-    <row r="366" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A366" s="6">
         <v>123464603</v>
       </c>
@@ -17272,7 +17237,7 @@
         <v>869773154</v>
       </c>
     </row>
-    <row r="367" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A367" s="6">
         <v>123465303</v>
       </c>
@@ -17313,7 +17278,7 @@
         <v>1931755636</v>
       </c>
     </row>
-    <row r="368" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A368" s="6">
         <v>123465602</v>
       </c>
@@ -17354,7 +17319,7 @@
         <v>1626537244</v>
       </c>
     </row>
-    <row r="369" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A369" s="6">
         <v>123465702</v>
       </c>
@@ -17395,7 +17360,7 @@
         <v>4138215333</v>
       </c>
     </row>
-    <row r="370" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A370" s="6">
         <v>123466103</v>
       </c>
@@ -17436,7 +17401,7 @@
         <v>1711080307</v>
       </c>
     </row>
-    <row r="371" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A371" s="6">
         <v>123466303</v>
       </c>
@@ -17477,7 +17442,7 @@
         <v>657180271</v>
       </c>
     </row>
-    <row r="372" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A372" s="6">
         <v>123466403</v>
       </c>
@@ -17518,7 +17483,7 @@
         <v>451604669</v>
       </c>
     </row>
-    <row r="373" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A373" s="6">
         <v>123467103</v>
       </c>
@@ -17559,7 +17524,7 @@
         <v>1993696289</v>
       </c>
     </row>
-    <row r="374" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A374" s="6">
         <v>123467203</v>
       </c>
@@ -17600,7 +17565,7 @@
         <v>1029828934</v>
       </c>
     </row>
-    <row r="375" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A375" s="6">
         <v>123467303</v>
       </c>
@@ -17641,7 +17606,7 @@
         <v>2506002544</v>
       </c>
     </row>
-    <row r="376" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A376" s="6">
         <v>123468303</v>
       </c>
@@ -17682,7 +17647,7 @@
         <v>1843227785</v>
       </c>
     </row>
-    <row r="377" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A377" s="6">
         <v>123468402</v>
       </c>
@@ -17723,7 +17688,7 @@
         <v>1847800676</v>
       </c>
     </row>
-    <row r="378" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A378" s="6">
         <v>123468503</v>
       </c>
@@ -17764,7 +17729,7 @@
         <v>843432897</v>
       </c>
     </row>
-    <row r="379" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A379" s="6">
         <v>123468603</v>
       </c>
@@ -17805,7 +17770,7 @@
         <v>861778297</v>
       </c>
     </row>
-    <row r="380" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A380" s="6">
         <v>123469303</v>
       </c>
@@ -17846,7 +17811,7 @@
         <v>3074685295</v>
       </c>
     </row>
-    <row r="381" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A381" s="6">
         <v>116471803</v>
       </c>
@@ -17887,7 +17852,7 @@
         <v>647671390</v>
       </c>
     </row>
-    <row r="382" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A382" s="6">
         <v>120480803</v>
       </c>
@@ -17928,7 +17893,7 @@
         <v>581067060</v>
       </c>
     </row>
-    <row r="383" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A383" s="6">
         <v>120481002</v>
       </c>
@@ -17969,7 +17934,7 @@
         <v>3318200394</v>
       </c>
     </row>
-    <row r="384" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A384" s="6">
         <v>120483302</v>
       </c>
@@ -18010,7 +17975,7 @@
         <v>1763060081</v>
       </c>
     </row>
-    <row r="385" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A385" s="6">
         <v>120484803</v>
       </c>
@@ -18051,7 +18016,7 @@
         <v>1148922406</v>
       </c>
     </row>
-    <row r="386" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A386" s="6">
         <v>120484903</v>
       </c>
@@ -18092,7 +18057,7 @@
         <v>1321535258</v>
       </c>
     </row>
-    <row r="387" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A387" s="6">
         <v>120485603</v>
       </c>
@@ -18133,7 +18098,7 @@
         <v>332111409</v>
       </c>
     </row>
-    <row r="388" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A388" s="6">
         <v>120486003</v>
       </c>
@@ -18174,7 +18139,7 @@
         <v>853692217</v>
       </c>
     </row>
-    <row r="389" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A389" s="6">
         <v>120488603</v>
       </c>
@@ -18215,7 +18180,7 @@
         <v>465104295</v>
       </c>
     </row>
-    <row r="390" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A390" s="6">
         <v>116493503</v>
       </c>
@@ -18256,7 +18221,7 @@
         <v>198219848</v>
       </c>
     </row>
-    <row r="391" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A391" s="6">
         <v>116495003</v>
       </c>
@@ -18297,7 +18262,7 @@
         <v>338454334</v>
       </c>
     </row>
-    <row r="392" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A392" s="6">
         <v>116495103</v>
       </c>
@@ -18338,7 +18303,7 @@
         <v>185893832</v>
       </c>
     </row>
-    <row r="393" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A393" s="6">
         <v>116496503</v>
       </c>
@@ -18379,7 +18344,7 @@
         <v>284253966</v>
       </c>
     </row>
-    <row r="394" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A394" s="6">
         <v>116496603</v>
       </c>
@@ -18420,7 +18385,7 @@
         <v>451144877</v>
       </c>
     </row>
-    <row r="395" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A395" s="6">
         <v>116498003</v>
       </c>
@@ -18461,7 +18426,7 @@
         <v>280423682</v>
       </c>
     </row>
-    <row r="396" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A396" s="6">
         <v>115503004</v>
       </c>
@@ -18502,7 +18467,7 @@
         <v>136003554</v>
       </c>
     </row>
-    <row r="397" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A397" s="6">
         <v>115504003</v>
       </c>
@@ -18543,7 +18508,7 @@
         <v>173578592</v>
       </c>
     </row>
-    <row r="398" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A398" s="6">
         <v>115506003</v>
       </c>
@@ -18584,7 +18549,7 @@
         <v>363042909</v>
       </c>
     </row>
-    <row r="399" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A399" s="6">
         <v>115508003</v>
       </c>
@@ -18625,7 +18590,7 @@
         <v>438577350</v>
       </c>
     </row>
-    <row r="400" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A400" s="6">
         <v>126515001</v>
       </c>
@@ -18666,7 +18631,7 @@
         <v>32328889201</v>
       </c>
     </row>
-    <row r="401" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A401" s="6">
         <v>120522003</v>
       </c>
@@ -18707,7 +18672,7 @@
         <v>522930062</v>
       </c>
     </row>
-    <row r="402" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A402" s="6">
         <v>119648303</v>
       </c>
@@ -18748,7 +18713,7 @@
         <v>504763632</v>
       </c>
     </row>
-    <row r="403" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A403" s="6">
         <v>109530304</v>
       </c>
@@ -18789,7 +18754,7 @@
         <v>20435951</v>
       </c>
     </row>
-    <row r="404" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A404" s="6">
         <v>109531304</v>
       </c>
@@ -18830,7 +18795,7 @@
         <v>115893416</v>
       </c>
     </row>
-    <row r="405" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A405" s="6">
         <v>109532804</v>
       </c>
@@ -18871,7 +18836,7 @@
         <v>39999431</v>
       </c>
     </row>
-    <row r="406" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A406" s="6">
         <v>109535504</v>
       </c>
@@ -18912,7 +18877,7 @@
         <v>58198754</v>
       </c>
     </row>
-    <row r="407" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A407" s="6">
         <v>109537504</v>
       </c>
@@ -18953,7 +18918,7 @@
         <v>41631143</v>
       </c>
     </row>
-    <row r="408" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A408" s="6">
         <v>129540803</v>
       </c>
@@ -18994,7 +18959,7 @@
         <v>609322122</v>
       </c>
     </row>
-    <row r="409" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A409" s="6">
         <v>129544503</v>
       </c>
@@ -19035,7 +19000,7 @@
         <v>131343789</v>
       </c>
     </row>
-    <row r="410" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A410" s="6">
         <v>129544703</v>
       </c>
@@ -19076,7 +19041,7 @@
         <v>166423061</v>
       </c>
     </row>
-    <row r="411" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A411" s="6">
         <v>129545003</v>
       </c>
@@ -19117,7 +19082,7 @@
         <v>322005421</v>
       </c>
     </row>
-    <row r="412" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A412" s="6">
         <v>129546003</v>
       </c>
@@ -19158,7 +19123,7 @@
         <v>275546798</v>
       </c>
     </row>
-    <row r="413" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A413" s="6">
         <v>129546103</v>
       </c>
@@ -19199,7 +19164,7 @@
         <v>420101715</v>
       </c>
     </row>
-    <row r="414" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A414" s="6">
         <v>129546803</v>
       </c>
@@ -19240,7 +19205,7 @@
         <v>110990377</v>
       </c>
     </row>
-    <row r="415" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A415" s="6">
         <v>129547303</v>
       </c>
@@ -19281,7 +19246,7 @@
         <v>210892527</v>
       </c>
     </row>
-    <row r="416" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A416" s="6">
         <v>129547203</v>
       </c>
@@ -19322,7 +19287,7 @@
         <v>106341668</v>
       </c>
     </row>
-    <row r="417" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A417" s="6">
         <v>129547603</v>
       </c>
@@ -19363,7 +19328,7 @@
         <v>352444666</v>
       </c>
     </row>
-    <row r="418" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A418" s="6">
         <v>129547803</v>
       </c>
@@ -19404,7 +19369,7 @@
         <v>165937548</v>
       </c>
     </row>
-    <row r="419" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A419" s="6">
         <v>129548803</v>
       </c>
@@ -19445,7 +19410,7 @@
         <v>137596160</v>
       </c>
     </row>
-    <row r="420" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A420" s="6">
         <v>116555003</v>
       </c>
@@ -19486,7 +19451,7 @@
         <v>342433405</v>
       </c>
     </row>
-    <row r="421" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A421" s="6">
         <v>116557103</v>
       </c>
@@ -19527,7 +19492,7 @@
         <v>501083287</v>
       </c>
     </row>
-    <row r="422" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A422" s="6">
         <v>108561003</v>
       </c>
@@ -19568,7 +19533,7 @@
         <v>120492437</v>
       </c>
     </row>
-    <row r="423" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A423" s="6">
         <v>108561803</v>
       </c>
@@ -19609,7 +19574,7 @@
         <v>168089692</v>
       </c>
     </row>
-    <row r="424" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A424" s="6">
         <v>108565203</v>
       </c>
@@ -19650,7 +19615,7 @@
         <v>126114293</v>
       </c>
     </row>
-    <row r="425" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A425" s="6">
         <v>108565503</v>
       </c>
@@ -19691,7 +19656,7 @@
         <v>158329015</v>
       </c>
     </row>
-    <row r="426" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A426" s="6">
         <v>108566303</v>
       </c>
@@ -19732,7 +19697,7 @@
         <v>133846343</v>
       </c>
     </row>
-    <row r="427" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A427" s="6">
         <v>108567004</v>
       </c>
@@ -19773,7 +19738,7 @@
         <v>46364649</v>
       </c>
     </row>
-    <row r="428" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A428" s="6">
         <v>108567204</v>
       </c>
@@ -19814,7 +19779,7 @@
         <v>60995765</v>
       </c>
     </row>
-    <row r="429" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A429" s="6">
         <v>108567404</v>
       </c>
@@ -19855,7 +19820,7 @@
         <v>71834439</v>
       </c>
     </row>
-    <row r="430" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A430" s="6">
         <v>108567703</v>
       </c>
@@ -19896,7 +19861,7 @@
         <v>400210608</v>
       </c>
     </row>
-    <row r="431" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A431" s="6">
         <v>108568404</v>
       </c>
@@ -19937,7 +19902,7 @@
         <v>44078734</v>
       </c>
     </row>
-    <row r="432" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A432" s="6">
         <v>108569103</v>
       </c>
@@ -19978,7 +19943,7 @@
         <v>180293637</v>
       </c>
     </row>
-    <row r="433" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A433" s="6">
         <v>117576303</v>
       </c>
@@ -20019,7 +19984,7 @@
         <v>123469596</v>
       </c>
     </row>
-    <row r="434" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A434" s="6">
         <v>119581003</v>
       </c>
@@ -20060,7 +20025,7 @@
         <v>111050741</v>
       </c>
     </row>
-    <row r="435" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A435" s="6">
         <v>119582503</v>
       </c>
@@ -20101,7 +20066,7 @@
         <v>187939018</v>
       </c>
     </row>
-    <row r="436" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A436" s="6">
         <v>119583003</v>
       </c>
@@ -20142,7 +20107,7 @@
         <v>113297981</v>
       </c>
     </row>
-    <row r="437" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="437" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A437" s="6">
         <v>119584503</v>
       </c>
@@ -20183,7 +20148,7 @@
         <v>217594678</v>
       </c>
     </row>
-    <row r="438" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A438" s="6">
         <v>119584603</v>
       </c>
@@ -20224,7 +20189,7 @@
         <v>226419807</v>
       </c>
     </row>
-    <row r="439" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A439" s="6">
         <v>119586503</v>
       </c>
@@ -20265,7 +20230,7 @@
         <v>96232166</v>
       </c>
     </row>
-    <row r="440" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A440" s="6">
         <v>117596003</v>
       </c>
@@ -20306,7 +20271,7 @@
         <v>181676670</v>
       </c>
     </row>
-    <row r="441" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A441" s="6">
         <v>117597003</v>
       </c>
@@ -20347,7 +20312,7 @@
         <v>273112825</v>
       </c>
     </row>
-    <row r="442" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="442" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A442" s="6">
         <v>117598503</v>
       </c>
@@ -20388,7 +20353,7 @@
         <v>232755825</v>
       </c>
     </row>
-    <row r="443" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="443" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A443" s="6">
         <v>116604003</v>
       </c>
@@ -20429,7 +20394,7 @@
         <v>552003361</v>
       </c>
     </row>
-    <row r="444" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="444" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A444" s="6">
         <v>116605003</v>
       </c>
@@ -20470,7 +20435,7 @@
         <v>352091035</v>
       </c>
     </row>
-    <row r="445" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="445" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A445" s="6">
         <v>106611303</v>
       </c>
@@ -20511,7 +20476,7 @@
         <v>182372652</v>
       </c>
     </row>
-    <row r="446" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A446" s="6">
         <v>106612203</v>
       </c>
@@ -20552,7 +20517,7 @@
         <v>271632475</v>
       </c>
     </row>
-    <row r="447" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A447" s="6">
         <v>106616203</v>
       </c>
@@ -20593,7 +20558,7 @@
         <v>236698776</v>
       </c>
     </row>
-    <row r="448" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A448" s="6">
         <v>106617203</v>
       </c>
@@ -20634,7 +20599,7 @@
         <v>221976085</v>
       </c>
     </row>
-    <row r="449" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A449" s="6">
         <v>106618603</v>
       </c>
@@ -20675,7 +20640,7 @@
         <v>114965076</v>
       </c>
     </row>
-    <row r="450" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A450" s="6">
         <v>105628302</v>
       </c>
@@ -20716,7 +20681,7 @@
         <v>664257287</v>
       </c>
     </row>
-    <row r="451" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A451" s="6">
         <v>101630504</v>
       </c>
@@ -20757,7 +20722,7 @@
         <v>107539400</v>
       </c>
     </row>
-    <row r="452" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A452" s="6">
         <v>101630903</v>
       </c>
@@ -20798,7 +20763,7 @@
         <v>188349763</v>
       </c>
     </row>
-    <row r="453" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A453" s="6">
         <v>101631003</v>
       </c>
@@ -20839,7 +20804,7 @@
         <v>182819407</v>
       </c>
     </row>
-    <row r="454" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A454" s="6">
         <v>101631203</v>
       </c>
@@ -20880,7 +20845,7 @@
         <v>226685518</v>
       </c>
     </row>
-    <row r="455" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A455" s="6">
         <v>101631503</v>
       </c>
@@ -20921,7 +20886,7 @@
         <v>147800625</v>
       </c>
     </row>
-    <row r="456" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A456" s="6">
         <v>101631703</v>
       </c>
@@ -20962,7 +20927,7 @@
         <v>1495261391</v>
       </c>
     </row>
-    <row r="457" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A457" s="6">
         <v>101631803</v>
       </c>
@@ -21003,7 +20968,7 @@
         <v>226336858</v>
       </c>
     </row>
-    <row r="458" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="458" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A458" s="6">
         <v>101631903</v>
       </c>
@@ -21044,7 +21009,7 @@
         <v>272877106</v>
       </c>
     </row>
-    <row r="459" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A459" s="6">
         <v>101632403</v>
       </c>
@@ -21085,7 +21050,7 @@
         <v>218863962</v>
       </c>
     </row>
-    <row r="460" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A460" s="6">
         <v>101633903</v>
       </c>
@@ -21126,7 +21091,7 @@
         <v>318440596</v>
       </c>
     </row>
-    <row r="461" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A461" s="6">
         <v>101636503</v>
       </c>
@@ -21167,7 +21132,7 @@
         <v>1563459364</v>
       </c>
     </row>
-    <row r="462" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="462" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A462" s="6">
         <v>101637002</v>
       </c>
@@ -21208,7 +21173,7 @@
         <v>556572810</v>
       </c>
     </row>
-    <row r="463" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A463" s="6">
         <v>101638003</v>
       </c>
@@ -21249,7 +21214,7 @@
         <v>785080219</v>
       </c>
     </row>
-    <row r="464" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A464" s="6">
         <v>101638803</v>
       </c>
@@ -21290,7 +21255,7 @@
         <v>249572092</v>
       </c>
     </row>
-    <row r="465" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A465" s="6">
         <v>119648703</v>
       </c>
@@ -21331,7 +21296,7 @@
         <v>409125307</v>
       </c>
     </row>
-    <row r="466" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A466" s="6">
         <v>119648903</v>
       </c>
@@ -21372,7 +21337,7 @@
         <v>316898468</v>
       </c>
     </row>
-    <row r="467" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="467" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A467" s="6">
         <v>107650603</v>
       </c>
@@ -21413,7 +21378,7 @@
         <v>477144634</v>
       </c>
     </row>
-    <row r="468" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A468" s="6">
         <v>107650703</v>
       </c>
@@ -21454,7 +21419,7 @@
         <v>382629048</v>
       </c>
     </row>
-    <row r="469" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="469" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A469" s="6">
         <v>107651603</v>
       </c>
@@ -21495,7 +21460,7 @@
         <v>330356125</v>
       </c>
     </row>
-    <row r="470" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A470" s="6">
         <v>107652603</v>
       </c>
@@ -21536,7 +21501,7 @@
         <v>1083309419</v>
       </c>
     </row>
-    <row r="471" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="471" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A471" s="6">
         <v>107653102</v>
       </c>
@@ -21577,7 +21542,7 @@
         <v>894018066</v>
       </c>
     </row>
-    <row r="472" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A472" s="6">
         <v>107653203</v>
       </c>
@@ -21618,7 +21583,7 @@
         <v>570284804</v>
       </c>
     </row>
-    <row r="473" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A473" s="6">
         <v>107653802</v>
       </c>
@@ -21659,7 +21624,7 @@
         <v>1349860172</v>
       </c>
     </row>
-    <row r="474" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A474" s="6">
         <v>107654103</v>
       </c>
@@ -21700,7 +21665,7 @@
         <v>148607622</v>
       </c>
     </row>
-    <row r="475" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="475" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A475" s="6">
         <v>107654403</v>
       </c>
@@ -21741,7 +21706,7 @@
         <v>666290661</v>
       </c>
     </row>
-    <row r="476" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="476" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A476" s="6">
         <v>107654903</v>
       </c>
@@ -21782,7 +21747,7 @@
         <v>442404811</v>
       </c>
     </row>
-    <row r="477" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="477" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A477" s="6">
         <v>107655803</v>
       </c>
@@ -21823,7 +21788,7 @@
         <v>111777108</v>
       </c>
     </row>
-    <row r="478" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A478" s="6">
         <v>107655903</v>
       </c>
@@ -21864,7 +21829,7 @@
         <v>410569594</v>
       </c>
     </row>
-    <row r="479" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="479" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A479" s="6">
         <v>107656303</v>
       </c>
@@ -21905,7 +21870,7 @@
         <v>287013491</v>
       </c>
     </row>
-    <row r="480" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="480" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A480" s="6">
         <v>107656502</v>
       </c>
@@ -21946,7 +21911,7 @@
         <v>1206785428</v>
       </c>
     </row>
-    <row r="481" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="481" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A481" s="6">
         <v>107657103</v>
       </c>
@@ -21987,7 +21952,7 @@
         <v>921377893</v>
       </c>
     </row>
-    <row r="482" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="482" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A482" s="6">
         <v>107657503</v>
       </c>
@@ -22028,7 +21993,7 @@
         <v>314061787</v>
       </c>
     </row>
-    <row r="483" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="483" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A483" s="6">
         <v>107658903</v>
       </c>
@@ -22069,7 +22034,7 @@
         <v>344282972</v>
       </c>
     </row>
-    <row r="484" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="484" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A484" s="6">
         <v>119665003</v>
       </c>
@@ -22110,7 +22075,7 @@
         <v>213175231</v>
       </c>
     </row>
-    <row r="485" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="485" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A485" s="6">
         <v>118667503</v>
       </c>
@@ -22151,7 +22116,7 @@
         <v>460520505</v>
       </c>
     </row>
-    <row r="486" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="486" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A486" s="6">
         <v>112671303</v>
       </c>
@@ -22192,7 +22157,7 @@
         <v>1324537858</v>
       </c>
     </row>
-    <row r="487" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="487" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A487" s="6">
         <v>112671603</v>
       </c>
@@ -22233,7 +22198,7 @@
         <v>1396907505</v>
       </c>
     </row>
-    <row r="488" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="488" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A488" s="6">
         <v>112671803</v>
       </c>
@@ -22274,7 +22239,7 @@
         <v>692287179</v>
       </c>
     </row>
-    <row r="489" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="489" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A489" s="6">
         <v>112672203</v>
       </c>
@@ -22315,7 +22280,7 @@
         <v>515667129</v>
       </c>
     </row>
-    <row r="490" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="490" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A490" s="6">
         <v>112672803</v>
       </c>
@@ -22356,7 +22321,7 @@
         <v>349799387</v>
       </c>
     </row>
-    <row r="491" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="491" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A491" s="6">
         <v>112674403</v>
       </c>
@@ -22397,7 +22362,7 @@
         <v>693288337</v>
       </c>
     </row>
-    <row r="492" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="492" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A492" s="6">
         <v>115674603</v>
       </c>
@@ -22438,7 +22403,7 @@
         <v>753037770</v>
       </c>
     </row>
-    <row r="493" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="493" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A493" s="6">
         <v>112675503</v>
       </c>
@@ -22479,7 +22444,7 @@
         <v>1029759940</v>
       </c>
     </row>
-    <row r="494" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="494" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A494" s="6">
         <v>112676203</v>
       </c>
@@ -22520,7 +22485,7 @@
         <v>581404492</v>
       </c>
     </row>
-    <row r="495" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="495" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A495" s="6">
         <v>112676403</v>
       </c>
@@ -22561,7 +22526,7 @@
         <v>852157710</v>
       </c>
     </row>
-    <row r="496" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="496" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A496" s="6">
         <v>112676503</v>
       </c>
@@ -22602,7 +22567,7 @@
         <v>700701714</v>
       </c>
     </row>
-    <row r="497" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="497" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A497" s="6">
         <v>112676703</v>
       </c>
@@ -22643,7 +22608,7 @@
         <v>850365258</v>
       </c>
     </row>
-    <row r="498" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="498" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A498" s="6">
         <v>115219002</v>
       </c>
@@ -22684,7 +22649,7 @@
         <v>2101662500</v>
       </c>
     </row>
-    <row r="499" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="499" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A499" s="6">
         <v>112678503</v>
       </c>
@@ -22725,7 +22690,7 @@
         <v>601228722</v>
       </c>
     </row>
-    <row r="500" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="500" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A500" s="6">
         <v>112679002</v>
       </c>
@@ -22766,7 +22731,7 @@
         <v>562886521</v>
       </c>
     </row>
-    <row r="501" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="501" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A501" s="6">
         <v>112679403</v>
       </c>
@@ -22807,7 +22772,7 @@
         <v>840452044</v>
       </c>
     </row>
-    <row r="503" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="503" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A503" s="11"/>
       <c r="B503" s="12"/>
       <c r="C503" s="12"/>
@@ -22871,6 +22836,31 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <SharedWithUsers xmlns="a7af8e22-4aad-4637-bdfe-8881feb25ebc">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010063A4E9D8B9AE294BB8664582FC3229C4" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2a2d9ea174ca71e18204fe09cb4b5ba8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="a7af8e22-4aad-4637-bdfe-8881feb25ebc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1e1d1e180fd2d7c84c724596e328884d" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -23027,39 +23017,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <SharedWithUsers xmlns="a7af8e22-4aad-4637-bdfe-8881feb25ebc">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73517AAA-83F8-45F9-BA38-871166B06847}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1180E27F-155F-47CC-83CE-711F11AFEEFC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="a7af8e22-4aad-4637-bdfe-8881feb25ebc"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{954D64FD-C931-4ABE-A76E-326067B5A485}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{954D64FD-C931-4ABE-A76E-326067B5A485}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1180E27F-155F-47CC-83CE-711F11AFEEFC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73517AAA-83F8-45F9-BA38-871166B06847}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="a7af8e22-4aad-4637-bdfe-8881feb25ebc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>